<commit_message>
Modified add patient form
</commit_message>
<xml_diff>
--- a/web-app/app/data/hospitals_list.xlsx
+++ b/web-app/app/data/hospitals_list.xlsx
@@ -1768,7 +1768,7 @@
     <t xml:space="preserve">РЕСПУБЛИКА:Казахстан ОБЛАСТЬ:АЛМАТИНСКАЯ ГОРОД ОБЛАСТНОГО ЗНАЧЕНИЯ:ТАЛДЫКОРГАН ПРОМЫШЛЕННАЯ ЗОНА:ЮЖНАЯ УЛИЦА:АЛМАЛЫ зд. 17</t>
   </si>
   <si>
-    <t xml:space="preserve">Алматы г.а.</t>
+    <t xml:space="preserve">г. Алматы</t>
   </si>
   <si>
     <t xml:space="preserve">Акционерно общество "Институт цифровой техники и технологий"</t>
@@ -12406,8 +12406,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1337" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1359" activeCellId="0" sqref="A1359"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A291" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A315" activeCellId="0" sqref="A315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added two more categories for Patient
</commit_message>
<xml_diff>
--- a/web-app/app/data/hospitals_list.xlsx
+++ b/web-app/app/data/hospitals_list.xlsx
@@ -6439,7 +6439,7 @@
     <t xml:space="preserve">РЕСПУБЛИКА:Казахстан ГОРОД РЕСПУБЛИКАНСКОГО ЗНАЧЕНИЯ:АСТАНА РАЙОН В ГОРОДЕ:САРЫАРКА УЛИЦА:ЖЕЛТОКСАН зд. 46</t>
   </si>
   <si>
-    <t xml:space="preserve">Республиканское государственное предприятие на праве хозяйственного ведения «Научно-исследовательский институт травматологии и ортопедии» Министерства здравоохранения Республики Казахстан</t>
+    <t xml:space="preserve">Республиканское государственное предприятие на праве хозяйственного ведения «НИИТО травматологии» Министерства здравоохранения Республики Казахстан</t>
   </si>
   <si>
     <t xml:space="preserve">РЕСПУБЛИКА:Казахстан ГОРОД РЕСПУБЛИКАНСКОГО ЗНАЧЕНИЯ:АСТАНА РАЙОН В ГОРОДЕ:АЛМАТЫ ПРОСПЕКТ:АБЫЛАЙ ХАНА зд. 15А</t>
@@ -12406,14 +12406,14 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A291" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A315" activeCellId="0" sqref="A315"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2828" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2848" activeCellId="0" sqref="A2848"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="67.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="145.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.14"/>
@@ -60821,6 +60821,25 @@
         <v>4093</v>
       </c>
     </row>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Finished optimizing import from .xls
</commit_message>
<xml_diff>
--- a/web-app/app/data/hospitals_list.xlsx
+++ b/web-app/app/data/hospitals_list.xlsx
@@ -4264,7 +4264,7 @@
     <t xml:space="preserve">РЕСПУБЛИКА:Казахстан ОБЛАСТЬ:АТЫРАУСКАЯ ГОРОД ОБЛАСТНОГО ЗНАЧЕНИЯ:АТЫРАУ УЛИЦА:АДМИРАЛ ЛЕВ ВЛАДИМИРСКИЙ д. 103</t>
   </si>
   <si>
-    <t xml:space="preserve">Восточно-Казахстанская область</t>
+    <t xml:space="preserve">Восточно-Казахстанская область (ВКО)</t>
   </si>
   <si>
     <t xml:space="preserve">Восточно-Казахстанский филиал Товарищество с ограниченной ответственностью Olymp Medical Group""</t>
@@ -8062,7 +8062,7 @@
     <t xml:space="preserve">Филиал Товарищество с ограниченной отвественностью "Научно-клинический центр кардиохирургии и трансплантологии" поликлиника "ZHANUYA"</t>
   </si>
   <si>
-    <t xml:space="preserve">Западно-Казахстанская область</t>
+    <t xml:space="preserve">Западно-Казахстанская область (ЗКО)</t>
   </si>
   <si>
     <t xml:space="preserve">Акционерное общество "Талап"</t>
@@ -11350,7 +11350,7 @@
     <t xml:space="preserve">Филиал Товарищество с ограниченной ответственностью "Centre Nova Diagnostic"</t>
   </si>
   <si>
-    <t xml:space="preserve">Северо-Казахстанская область</t>
+    <t xml:space="preserve">Северо-Казахстанская область (СКО)</t>
   </si>
   <si>
     <t xml:space="preserve">Индивидуальный предприниматель "PROFIT"</t>
@@ -12406,13 +12406,13 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2828" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2848" activeCellId="0" sqref="A2848"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1194" activeCellId="0" sqref="A987:A1211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="145.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.72"/>

</xml_diff>